<commit_message>
commit Jostens BrowserStack Test Suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/jostens/qa/testdata/Jostens-backup.xlsx
+++ b/src/main/java/com/jostens/qa/testdata/Jostens-backup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CE308C02-4E1E-43A5-A163-7D8CCED87077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{59BF00EF-0D97-4374-B8E6-AC3D4314D1CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21990" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21960" windowHeight="16500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Payment" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q21"/>
+  <oleSize ref="A1:X21"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="634">
   <si>
     <t>Website</t>
   </si>
@@ -352,6 +352,39 @@
     <t>MorningsideMustang124</t>
   </si>
   <si>
+    <t>Failure - 2020/12/13 08:52:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:52:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:52:14</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 08:52:15</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:52:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:53:06</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:53:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:53:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:53:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:53:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 08:53:58</t>
+  </si>
+  <si>
     <t>Success - 2020/12/13 08:54:02</t>
   </si>
   <si>
@@ -361,6 +394,9 @@
     <t>Cardholder Name</t>
   </si>
   <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
     <t>Security Code</t>
   </si>
   <si>
@@ -373,175 +409,1525 @@
     <t>Cynthia Ambrosia</t>
   </si>
   <si>
+    <t>0223</t>
+  </si>
+  <si>
     <t>096</t>
   </si>
   <si>
     <t>Invalid CC Number</t>
   </si>
   <si>
+    <t>Success - 2020/12/13 09:53:34</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:53:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:53:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:53:43</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:54:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:54:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:54:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:54:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:55:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:55:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:55:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:55:22</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 09:55:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:56:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:56:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:56:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:56:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:57:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:57:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:03</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:06</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:28</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 09:58:37</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 09:58:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:00:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:00:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:00:16</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:00:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:00:46</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:01:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:01:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:01:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:01:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:01:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:02:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:02:02</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:02:06</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:03:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:03:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:03:56</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:04:00</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:04:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:04:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:26</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:33</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:43</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:05:44</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:05:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:09:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:09:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:09:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:09:14</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:09:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:10:51</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:11:03</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:11:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:11:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:11:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:11:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:12:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:12:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:03</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:13:30</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:13:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:14:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:14:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:14:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:14:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:15:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:15:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:28</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:16:36</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:17:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:22:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:22:26</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:22:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:22:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:22:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:23:18</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:23:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:23:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:23:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:23:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:24:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:24:08</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:24:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:33:28</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:33:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:33:34</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:33:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:34:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:34:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:34:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:34:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:34:56</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:35:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:35:16</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:35:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:39:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:39:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:39:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:39:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:40:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:40:34</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:40:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:40:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:41:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:41:18</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:41:26</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:41:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:54:02</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:54:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:54:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:54:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:54:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:54:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:55:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:55:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:55:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:55:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:56:00</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:56:01</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 10:56:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:57:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:57:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:57:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:58:00</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:58:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:58:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:59:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:59:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:59:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:59:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:59:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 10:59:37</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:00:02</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:01:26</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:01:30</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:01:33</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:01:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:02:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:02:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:02:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:02:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:03:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:03:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:03:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:03:22</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:03:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:11:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:11:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:11:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:11:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:11:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:12:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:12:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:12:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:12:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:12:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:12:55</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:13:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:14:43</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:14:46</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:14:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:14:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:15:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:15:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:16:00</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:16:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:16:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:16:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:16:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:16:30</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:16:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:18:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:18:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:18:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:18:53</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:19:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:19:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:20:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:20:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:20:15</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:20:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:20:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:20:32</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:20:43</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:22:39</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:22:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:22:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:22:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:23:14</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:23:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:23:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:23:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:24:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:24:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:24:28</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:24:29</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:24:40</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:26:03</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:26:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:26:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:26:12</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:26:37</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:26:50</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:27:23</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 11:27:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:27:30</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:27:33</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:27:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:28:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:28:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:28:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:28:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:29:03</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:29:14</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:29:15</t>
+  </si>
+  <si>
     <t>Failure - 2020/12/13 11:29:28</t>
   </si>
   <si>
-    <t>Success - 2020/12/14 14:40:12</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:40:19</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:40:23</t>
-  </si>
-  <si>
-    <t>Failure - 2020/12/14 14:40:25</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:40:58</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:41:19</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:41:41</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:41:43</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:41:55</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:42:03</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:42:12</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:42:23</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:45:55</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:46:00</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:46:03</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:46:07</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:46:36</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:46:56</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:17</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:19</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:20</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:30</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:37</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:45</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:46</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/14 14:47:56</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:26:19</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:26:24</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:26:27</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:26:30</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:26:55</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:27:16</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:27:37</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:27:39</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:27:40</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:27:50</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:28:01</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:28:12</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:28:13</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/18 10:28:23</t>
-  </si>
-  <si>
-    <t>Failure - 2020/12/19 02:24:42</t>
-  </si>
-  <si>
-    <t>Failure - 2020/12/19 02:24:47</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:24:51</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:24:54</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:25:22</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:25:43</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:04</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:06</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:07</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:17</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:28</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:35</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:36</t>
-  </si>
-  <si>
-    <t>Success - 2020/12/19 02:26:46</t>
+    <t>Success - 2020/12/13 11:33:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:33:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:33:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:33:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:33:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:33:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:34:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:34:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:34:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:34:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:34:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:34:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:35:00</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:54:14</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:54:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:54:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:54:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:54:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:55:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:55:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:55:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:55:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:55:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:55:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 11:56:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:04:19</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 12:04:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:04:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:04:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:04:53</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:05:16</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:05:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:05:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:05:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:06:00</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 12:06:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:06:14</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 12:06:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:11:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:11:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:11:56</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:11:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:12:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:12:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:33</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:13:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:38:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:38:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:38:38</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:38:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:39:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:39:30</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:39:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:39:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:39:53</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:40:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:40:15</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:40:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:40:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:40:33</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 12:46:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:46:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:46:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:46:26</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:46:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:47:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:47:34</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:47:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:47:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:47:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:47:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:48:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:48:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:48:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:59:38</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:59:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:59:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 12:59:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:00:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:00:34</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:00:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:00:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:00:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:01:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:01:16</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:01:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:01:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:01:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:08:16</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:08:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:08:26</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:08:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:08:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:09:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:09:38</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:09:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:09:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:10:03</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:10:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:10:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:10:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:17:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:18:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:18:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:18:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:18:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:18:56</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:19:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:19:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:19:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:19:38</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:19:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:19:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:20:03</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:22:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:22:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:22:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:23:00</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:23:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:23:46</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:28</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:24:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:35:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:35:30</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:35:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:35:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:37:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:37:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:37:16</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:37:22</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 13:37:53</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 13:38:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:39:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:39:13</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:39:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:39:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:39:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:40:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:40:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:40:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:40:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:41:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:41:25</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:41:43</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:42:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:42:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:42:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:42:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:42:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:49:19</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:49:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:49:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:49:38</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:50:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:50:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:51:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:51:06</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:51:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:51:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:51:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:51:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:52:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:52:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:52:14</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:52:17</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 13:52:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:25:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:25:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:25:15</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:25:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:25:53</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:26:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:26:51</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:26:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:26:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:26:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:27:20</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:27:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:27:56</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:27:57</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:27:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:28:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:28:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:41:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:41:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:41:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:42:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:42:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:43:05</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:43:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:43:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:43:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:43:38</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:44:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:44:23</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:44:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:44:46</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:44:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:44:49</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 14:45:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:03:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:03:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:03:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:04:07</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:04:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:05:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:05:35</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:05:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:05:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:05:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:06:06</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:06:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:06:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:06:46</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:06:47</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:06:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:07:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:43:55</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:44:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:44:08</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:44:14</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 15:44:47</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 15:45:02</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 15:45:17</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 15:45:21</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 15:45:23</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/13 15:45:24</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:45:50</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:46:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:46:29</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:46:30</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:46:31</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:46:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:46:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:47:52</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:47:58</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:48:04</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:48:10</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:48:43</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:49:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:49:37</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:49:42</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:49:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:49:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:06</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:22</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:41</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:43</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:44</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:45</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/13 15:50:59</t>
   </si>
 </sst>
 </file>
@@ -874,7 +2260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -934,7 +2320,7 @@
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>617</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -957,7 +2343,7 @@
         <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>618</v>
       </c>
     </row>
   </sheetData>
@@ -992,7 +2378,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,7 +2389,7 @@
         <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1014,7 +2400,7 @@
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -1108,7 +2494,7 @@
         <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>162</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1143,7 +2529,7 @@
         <v>82</v>
       </c>
       <c r="K3" t="s">
-        <v>163</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1178,7 +2564,7 @@
         <v>82</v>
       </c>
       <c r="K4" t="s">
-        <v>164</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +2632,7 @@
         <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>165</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1269,7 +2655,7 @@
         <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>165</v>
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1292,7 +2678,7 @@
         <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -1423,7 +2809,7 @@
         <v>53</v>
       </c>
       <c r="P2" t="s">
-        <v>167</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1473,7 +2859,7 @@
         <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>168</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1523,7 +2909,7 @@
         <v>53</v>
       </c>
       <c r="P4" t="s">
-        <v>170</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -1540,7 +2926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAE82A9-403E-41ED-A26F-7AD33462531D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1554,19 +2940,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>371</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -1574,19 +2960,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>171</v>
+        <v>633</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>